<commit_message>
fix glyphs in MoClo-YTK submission excel file
</commit_message>
<xml_diff>
--- a/submissions/kits-moclo-ytk/submission.xlsx
+++ b/submissions/kits-moclo-ytk/submission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/Documents/Projects/ShareYourCloning/ShareYourCloning-submission/submissions/kits-moclo-ytk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1405894-7CD0-174C-8693-8457E5A201EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251B87D-075F-AA43-ADBE-CB7A24E66D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="500" windowWidth="22780" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3705,7 +3705,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2" t="s">
-        <v>447</v>
+        <v>404</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -4273,7 +4273,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>404</v>
+        <v>448</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>

</xml_diff>

<commit_message>
fix glyphs in MoClo-YTK submission excel file (#66)
</commit_message>
<xml_diff>
--- a/submissions/kits-moclo-ytk/submission.xlsx
+++ b/submissions/kits-moclo-ytk/submission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/Documents/Projects/ShareYourCloning/ShareYourCloning-submission/submissions/kits-moclo-ytk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1405894-7CD0-174C-8693-8457E5A201EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7251B87D-075F-AA43-ADBE-CB7A24E66D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="500" windowWidth="22780" windowHeight="21460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3705,7 +3705,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2" t="s">
-        <v>447</v>
+        <v>404</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -4273,7 +4273,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>404</v>
+        <v>448</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>

</xml_diff>